<commit_message>
2021-04-20 18:07:53 - Update
</commit_message>
<xml_diff>
--- a/2021-04-20.swap.xlsx
+++ b/2021-04-20.swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4246,6 +4246,56 @@
         <v>42308</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" s="2">
+        <v>44306</v>
+      </c>
+      <c r="B78">
+        <v>820</v>
+      </c>
+      <c r="C78">
+        <v>3406</v>
+      </c>
+      <c r="D78">
+        <v>300</v>
+      </c>
+      <c r="E78">
+        <v>5259</v>
+      </c>
+      <c r="F78">
+        <v>203</v>
+      </c>
+      <c r="G78">
+        <v>1816</v>
+      </c>
+      <c r="H78">
+        <v>1000</v>
+      </c>
+      <c r="I78">
+        <v>28500</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>3517</v>
+      </c>
+      <c r="N78">
+        <v>140</v>
+      </c>
+      <c r="O78">
+        <v>950</v>
+      </c>
+      <c r="P78">
+        <v>42498</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>